<commit_message>
Aplicando paginacion a la vista
</commit_message>
<xml_diff>
--- a/backup/cuenta_2200555154.xlsx
+++ b/backup/cuenta_2200555154.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="76">
   <si>
     <t>  TRANSFERENCIA INTERNET</t>
   </si>
@@ -234,6 +234,24 @@
   </si>
   <si>
     <t>4014.30</t>
+  </si>
+  <si>
+    <t>0000950378</t>
+  </si>
+  <si>
+    <t>0000950389</t>
+  </si>
+  <si>
+    <t>0000950666</t>
+  </si>
+  <si>
+    <t>4015.55</t>
+  </si>
+  <si>
+    <t>4014.80</t>
+  </si>
+  <si>
+    <t>4014.55</t>
   </si>
 </sst>
 </file>
@@ -556,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H1" sqref="H1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +589,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>41681</v>
+        <v>41684</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -580,25 +598,25 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H1" t="str">
-        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd H:m:s"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL 'mo_borrado_logico' =&gt; false),")</f>
-        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-11'), 'mo_concepto' =&gt; 'INTERES A SU FAVOR', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000950673', 'mo_oficina' =&gt; 'AGENCIA PARA PROCESOS BATCH', 'mo_monto' =&gt; 0.25  , 'mo_saldo' =&gt; 4014.30, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-12 22:34:41'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL 'mo_borrado_logico' =&gt; false),</v>
+        <f ca="1">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A1,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B1,"', 'mo_tipo' =&gt; '",C1,"', 'mo_documento' =&gt; '",D1,"', 'mo_oficina' =&gt; '",E1,"', 'mo_monto' =&gt; ",F1,", 'mo_saldo' =&gt; ",G1,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd HH:mm:ss"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-14'), 'mo_concepto' =&gt; 'INTERES A SU FAVOR', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000950378', 'mo_oficina' =&gt; 'AGENCIA PARA PROCESOS BATCH', 'mo_monto' =&gt; 0.75  , 'mo_saldo' =&gt; 4015.55, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-17 21:14:23'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>41680</v>
+        <v>41683</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -607,7 +625,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -616,12 +634,16 @@
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H3" ca="1" si="0">CONCATENATE("array('mo_fecha' =&gt; new \DateTime('",TEXT(A2,"yyyy-mm-dd"),"'), 'mo_concepto' =&gt; '",B2,"', 'mo_tipo' =&gt; '",C2,"', 'mo_documento' =&gt; '",D2,"', 'mo_oficina' =&gt; '",E2,"', 'mo_monto' =&gt; ",F2,", 'mo_saldo' =&gt; ",G2,", 'mo_fecha_crea' =&gt; new \DateTime('",TEXT(NOW(),"yyyy-mm-dd HH:mm:ss"),"'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),")</f>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-13'), 'mo_concepto' =&gt; 'INTERES A SU FAVOR', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000950389', 'mo_oficina' =&gt; 'AGENCIA PARA PROCESOS BATCH', 'mo_monto' =&gt; 0.25  , 'mo_saldo' =&gt; 4014.80, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-17 21:14:23'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>41677</v>
+        <v>41682</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -630,21 +652,25 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>array('mo_fecha' =&gt; new \DateTime('2014-02-12'), 'mo_concepto' =&gt; 'INTERES A SU FAVOR', 'mo_tipo' =&gt; 'C', 'mo_documento' =&gt; '0000950666', 'mo_oficina' =&gt; 'AGENCIA PARA PROCESOS BATCH', 'mo_monto' =&gt; 0.25  , 'mo_saldo' =&gt; 4014.55, 'mo_fecha_crea' =&gt; new \DateTime('2014-02-17 21:14:23'), 'mo_quien_crea' =&gt; 1, 'mo_fecha_modifica' =&gt; NULL, 'mo_quien_modifica' =&gt; NULL, 'mo_borrado_logico' =&gt; false),</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>41676</v>
+        <v>41681</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -653,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -662,12 +688,12 @@
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>41675</v>
+        <v>41680</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -676,7 +702,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -685,12 +711,12 @@
         <v>10</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>41674</v>
+        <v>41677</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -699,44 +725,44 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>41674</v>
+        <v>41676</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>41673</v>
+        <v>41675</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -745,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
@@ -754,12 +780,12 @@
         <v>10</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>41670</v>
+        <v>41674</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -768,44 +794,44 @@
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
         <v>4</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>41669</v>
+        <v>41674</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>41668</v>
+        <v>41673</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -814,7 +840,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
@@ -823,12 +849,12 @@
         <v>10</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>41667</v>
+        <v>41670</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -837,21 +863,21 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
         <v>4</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>41666</v>
+        <v>41669</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
@@ -860,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
         <v>4</v>
@@ -869,35 +895,35 @@
         <v>10</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>41666</v>
+        <v>41668</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>41663</v>
+        <v>41667</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -906,21 +932,21 @@
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>41662</v>
+        <v>41666</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -929,44 +955,44 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E16" t="s">
         <v>4</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>41661</v>
+        <v>41666</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>41660</v>
+        <v>41663</v>
       </c>
       <c r="B18" t="s">
         <v>3</v>
@@ -975,21 +1001,21 @@
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
         <v>4</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>41659</v>
+        <v>41662</v>
       </c>
       <c r="B19" t="s">
         <v>3</v>
@@ -1007,12 +1033,12 @@
         <v>16</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>41656</v>
+        <v>41661</v>
       </c>
       <c r="B20" t="s">
         <v>3</v>
@@ -1027,15 +1053,15 @@
         <v>4</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>41655</v>
+        <v>41660</v>
       </c>
       <c r="B21" t="s">
         <v>3</v>
@@ -1053,12 +1079,12 @@
         <v>16</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>41654</v>
+        <v>41659</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -1067,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E22" t="s">
         <v>4</v>
@@ -1076,12 +1102,12 @@
         <v>16</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>41653</v>
+        <v>41656</v>
       </c>
       <c r="B23" t="s">
         <v>3</v>
@@ -1090,21 +1116,21 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E23" t="s">
         <v>4</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>41652</v>
+        <v>41655</v>
       </c>
       <c r="B24" t="s">
         <v>3</v>
@@ -1113,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E24" t="s">
         <v>4</v>
@@ -1122,35 +1148,35 @@
         <v>16</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>41652</v>
+        <v>41654</v>
       </c>
       <c r="B25" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E25" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>41649</v>
+        <v>41653</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
@@ -1159,21 +1185,21 @@
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>41648</v>
+        <v>41652</v>
       </c>
       <c r="B27" t="s">
         <v>3</v>
@@ -1182,44 +1208,44 @@
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E27" t="s">
         <v>4</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>41647</v>
+        <v>41652</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>41646</v>
+        <v>41649</v>
       </c>
       <c r="B29" t="s">
         <v>3</v>
@@ -1228,21 +1254,21 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E29" t="s">
         <v>4</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>41645</v>
+        <v>41648</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
@@ -1251,7 +1277,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="E30" t="s">
         <v>4</v>
@@ -1260,12 +1286,12 @@
         <v>24</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>41642</v>
+        <v>41647</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
@@ -1274,21 +1300,21 @@
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E31" t="s">
         <v>4</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>41641</v>
+        <v>41646</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
@@ -1297,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E32" t="s">
         <v>4</v>
@@ -1306,20 +1332,89 @@
         <v>24</v>
       </c>
       <c r="G32" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>